<commit_message>
BME680 sensor added to the system
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2259" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5419" uniqueCount="154">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -343,6 +343,141 @@
   </si>
   <si>
     <t xml:space="preserve">0123456789 :APM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ScrollWhellTxt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ariblk.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;val&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menu Element: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pressure:&lt;value&gt;%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IAQ:&lt;value&gt;%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId92</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature:&lt;value&gt;&lt;'223'&gt;C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pressure:&lt;value&gt;mmHg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2 Concentration:&lt;value&gt;ppm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature:&lt;value&gt; C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Humidity:&lt;value&gt; %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pressure:&lt;value&gt; mmHg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2 Concentration:&lt;value&gt; ppm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature:&lt;value&gt; °C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature: &lt;value&gt;°C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Humidity: &lt;value&gt;%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pressure: &lt;value&gt;mmHg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2 Concentration: &lt;value&gt;ppm</t>
   </si>
 </sst>
 </file>
@@ -1574,6 +1709,33 @@
       </c>
     </row>
     <row r="8" spans="2:16">
+      <c r="B8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" t="s">
+        <v>40</v>
+      </c>
       <c r="L8" s="7" t="s">
         <v>8</v>
       </c>
@@ -1735,7 +1897,7 @@
         <v>46</v>
       </c>
       <c r="F6" t="s">
-        <v>57</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="2:6">
@@ -1990,7 +2152,7 @@
         <v>46</v>
       </c>
       <c r="F21" t="s">
-        <v>86</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="2:6">
@@ -2503,7 +2665,482 @@
         <v>47</v>
       </c>
     </row>
-    <row r="52"/>
+    <row r="52">
+      <c r="B52" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52" t="s">
+        <v>38</v>
+      </c>
+      <c r="D52" t="s">
+        <v>48</v>
+      </c>
+      <c r="E52" t="s">
+        <v>46</v>
+      </c>
+      <c r="F52" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="B53" t="s">
+        <v>112</v>
+      </c>
+      <c r="C53" t="s">
+        <v>38</v>
+      </c>
+      <c r="D53" t="s">
+        <v>48</v>
+      </c>
+      <c r="E53" t="s">
+        <v>46</v>
+      </c>
+      <c r="F53" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="B54" t="s">
+        <v>114</v>
+      </c>
+      <c r="C54" t="s">
+        <v>38</v>
+      </c>
+      <c r="D54" t="s">
+        <v>48</v>
+      </c>
+      <c r="E54" t="s">
+        <v>46</v>
+      </c>
+      <c r="F54" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="B55" t="s">
+        <v>116</v>
+      </c>
+      <c r="C55" t="s">
+        <v>38</v>
+      </c>
+      <c r="D55" t="s">
+        <v>48</v>
+      </c>
+      <c r="E55" t="s">
+        <v>46</v>
+      </c>
+      <c r="F55" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="B56" t="s">
+        <v>117</v>
+      </c>
+      <c r="C56" t="s">
+        <v>38</v>
+      </c>
+      <c r="D56" t="s">
+        <v>45</v>
+      </c>
+      <c r="E56" t="s">
+        <v>46</v>
+      </c>
+      <c r="F56" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57" t="s">
+        <v>118</v>
+      </c>
+      <c r="C57" t="s">
+        <v>38</v>
+      </c>
+      <c r="D57" t="s">
+        <v>45</v>
+      </c>
+      <c r="E57" t="s">
+        <v>46</v>
+      </c>
+      <c r="F57" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" t="s">
+        <v>119</v>
+      </c>
+      <c r="C58" t="s">
+        <v>38</v>
+      </c>
+      <c r="D58" t="s">
+        <v>45</v>
+      </c>
+      <c r="E58" t="s">
+        <v>46</v>
+      </c>
+      <c r="F58" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" t="s">
+        <v>120</v>
+      </c>
+      <c r="C59" t="s">
+        <v>38</v>
+      </c>
+      <c r="D59" t="s">
+        <v>45</v>
+      </c>
+      <c r="E59" t="s">
+        <v>46</v>
+      </c>
+      <c r="F59" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="B60" t="s">
+        <v>121</v>
+      </c>
+      <c r="C60" t="s">
+        <v>38</v>
+      </c>
+      <c r="D60" t="s">
+        <v>45</v>
+      </c>
+      <c r="E60" t="s">
+        <v>46</v>
+      </c>
+      <c r="F60" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="B61" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61" t="s">
+        <v>38</v>
+      </c>
+      <c r="D61" t="s">
+        <v>45</v>
+      </c>
+      <c r="E61" t="s">
+        <v>46</v>
+      </c>
+      <c r="F61" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62" t="s">
+        <v>123</v>
+      </c>
+      <c r="C62" t="s">
+        <v>38</v>
+      </c>
+      <c r="D62" t="s">
+        <v>45</v>
+      </c>
+      <c r="E62" t="s">
+        <v>46</v>
+      </c>
+      <c r="F62" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="B63" t="s">
+        <v>124</v>
+      </c>
+      <c r="C63" t="s">
+        <v>38</v>
+      </c>
+      <c r="D63" t="s">
+        <v>45</v>
+      </c>
+      <c r="E63" t="s">
+        <v>46</v>
+      </c>
+      <c r="F63" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64" t="s">
+        <v>125</v>
+      </c>
+      <c r="C64" t="s">
+        <v>38</v>
+      </c>
+      <c r="D64" t="s">
+        <v>45</v>
+      </c>
+      <c r="E64" t="s">
+        <v>46</v>
+      </c>
+      <c r="F64" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65" t="s">
+        <v>126</v>
+      </c>
+      <c r="C65" t="s">
+        <v>38</v>
+      </c>
+      <c r="D65" t="s">
+        <v>45</v>
+      </c>
+      <c r="E65" t="s">
+        <v>46</v>
+      </c>
+      <c r="F65" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66" t="s">
+        <v>127</v>
+      </c>
+      <c r="C66" t="s">
+        <v>38</v>
+      </c>
+      <c r="D66" t="s">
+        <v>45</v>
+      </c>
+      <c r="E66" t="s">
+        <v>46</v>
+      </c>
+      <c r="F66" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="B67" t="s">
+        <v>128</v>
+      </c>
+      <c r="C67" t="s">
+        <v>38</v>
+      </c>
+      <c r="D67" t="s">
+        <v>48</v>
+      </c>
+      <c r="E67" t="s">
+        <v>46</v>
+      </c>
+      <c r="F67" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="B68" t="s">
+        <v>130</v>
+      </c>
+      <c r="C68" t="s">
+        <v>38</v>
+      </c>
+      <c r="D68" t="s">
+        <v>48</v>
+      </c>
+      <c r="E68" t="s">
+        <v>46</v>
+      </c>
+      <c r="F68" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="B69" t="s">
+        <v>131</v>
+      </c>
+      <c r="C69" t="s">
+        <v>38</v>
+      </c>
+      <c r="D69" t="s">
+        <v>45</v>
+      </c>
+      <c r="E69" t="s">
+        <v>46</v>
+      </c>
+      <c r="F69" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70" t="s">
+        <v>132</v>
+      </c>
+      <c r="C70" t="s">
+        <v>38</v>
+      </c>
+      <c r="D70" t="s">
+        <v>45</v>
+      </c>
+      <c r="E70" t="s">
+        <v>46</v>
+      </c>
+      <c r="F70" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71" t="s">
+        <v>133</v>
+      </c>
+      <c r="C71" t="s">
+        <v>38</v>
+      </c>
+      <c r="D71" t="s">
+        <v>45</v>
+      </c>
+      <c r="E71" t="s">
+        <v>46</v>
+      </c>
+      <c r="F71" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="B72" t="s">
+        <v>134</v>
+      </c>
+      <c r="C72" t="s">
+        <v>38</v>
+      </c>
+      <c r="D72" t="s">
+        <v>45</v>
+      </c>
+      <c r="E72" t="s">
+        <v>46</v>
+      </c>
+      <c r="F72" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" t="s">
+        <v>135</v>
+      </c>
+      <c r="C73" t="s">
+        <v>38</v>
+      </c>
+      <c r="D73" t="s">
+        <v>45</v>
+      </c>
+      <c r="E73" t="s">
+        <v>46</v>
+      </c>
+      <c r="F73" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="B74" t="s">
+        <v>136</v>
+      </c>
+      <c r="C74" t="s">
+        <v>38</v>
+      </c>
+      <c r="D74" t="s">
+        <v>45</v>
+      </c>
+      <c r="E74" t="s">
+        <v>46</v>
+      </c>
+      <c r="F74" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="B75" t="s">
+        <v>137</v>
+      </c>
+      <c r="C75" t="s">
+        <v>38</v>
+      </c>
+      <c r="D75" t="s">
+        <v>45</v>
+      </c>
+      <c r="E75" t="s">
+        <v>46</v>
+      </c>
+      <c r="F75" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="B76" t="s">
+        <v>138</v>
+      </c>
+      <c r="C76" t="s">
+        <v>38</v>
+      </c>
+      <c r="D76" t="s">
+        <v>45</v>
+      </c>
+      <c r="E76" t="s">
+        <v>46</v>
+      </c>
+      <c r="F76" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="B77" t="s">
+        <v>139</v>
+      </c>
+      <c r="C77" t="s">
+        <v>38</v>
+      </c>
+      <c r="D77" t="s">
+        <v>45</v>
+      </c>
+      <c r="E77" t="s">
+        <v>46</v>
+      </c>
+      <c r="F77" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="B78" t="s">
+        <v>140</v>
+      </c>
+      <c r="C78" t="s">
+        <v>38</v>
+      </c>
+      <c r="D78" t="s">
+        <v>45</v>
+      </c>
+      <c r="E78" t="s">
+        <v>46</v>
+      </c>
+      <c r="F78" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="B79" t="s">
+        <v>141</v>
+      </c>
+      <c r="C79" t="s">
+        <v>38</v>
+      </c>
+      <c r="D79" t="s">
+        <v>45</v>
+      </c>
+      <c r="E79" t="s">
+        <v>46</v>
+      </c>
+      <c r="F79" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Lags removed, signals smoothing added
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5419" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7197" uniqueCount="155">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -478,6 +478,9 @@
   </si>
   <si>
     <t xml:space="preserve">CO2 Concentration: &lt;value&gt;ppm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">700.54&lt;value&gt;</t>
   </si>
 </sst>
 </file>
@@ -1953,7 +1956,7 @@
     </row>
     <row r="10" spans="2:6">
       <c r="B10" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
         <v>38</v>
@@ -1970,7 +1973,7 @@
     </row>
     <row r="11" spans="2:6">
       <c r="B11" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C11" t="s">
         <v>38</v>
@@ -1982,46 +1985,46 @@
         <v>46</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C12" t="s">
         <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E12" t="s">
         <v>46</v>
       </c>
       <c r="F12" t="s">
-        <v>49</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C13" t="s">
         <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
         <v>46</v>
       </c>
       <c r="F13" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
@@ -2038,7 +2041,7 @@
     </row>
     <row r="15" spans="2:6">
       <c r="B15" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
         <v>38</v>
@@ -2055,30 +2058,30 @@
     </row>
     <row r="16" spans="2:6">
       <c r="B16" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="C16" t="s">
         <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E16" t="s">
         <v>46</v>
       </c>
       <c r="F16" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="2:6">
       <c r="B17" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E17" t="s">
         <v>46</v>
@@ -2089,58 +2092,58 @@
     </row>
     <row r="18" spans="2:6">
       <c r="B18" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="C18" t="s">
         <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
         <v>46</v>
       </c>
       <c r="F18" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="2:6">
       <c r="B19" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="C19" t="s">
         <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E19" t="s">
         <v>46</v>
       </c>
       <c r="F19" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="2:6">
       <c r="B20" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="C20" t="s">
         <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E20" t="s">
         <v>46</v>
       </c>
       <c r="F20" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="2:6">
       <c r="B21" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="C21" t="s">
         <v>38</v>
@@ -2152,12 +2155,12 @@
         <v>46</v>
       </c>
       <c r="F21" t="s">
-        <v>151</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="2:6">
       <c r="B22" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="C22" t="s">
         <v>38</v>
@@ -2169,52 +2172,52 @@
         <v>46</v>
       </c>
       <c r="F22" t="s">
-        <v>59</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="2:6">
       <c r="B23" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="C23" t="s">
         <v>38</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E23" t="s">
         <v>46</v>
       </c>
       <c r="F23" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="2:6">
       <c r="B24" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="C24" t="s">
         <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E24" t="s">
         <v>46</v>
       </c>
       <c r="F24" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="2:6">
       <c r="B25" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="C25" t="s">
         <v>38</v>
       </c>
       <c r="D25" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E25" t="s">
         <v>46</v>
@@ -2225,143 +2228,143 @@
     </row>
     <row r="26" spans="2:6">
       <c r="B26" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="C26" t="s">
         <v>38</v>
       </c>
       <c r="D26" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E26" t="s">
         <v>46</v>
       </c>
       <c r="F26" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="2:6">
       <c r="B27" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="C27" t="s">
         <v>38</v>
       </c>
       <c r="D27" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E27" t="s">
         <v>46</v>
       </c>
       <c r="F27" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="2:6">
       <c r="B28" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C28" t="s">
         <v>38</v>
       </c>
       <c r="D28" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E28" t="s">
         <v>46</v>
       </c>
       <c r="F28" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="2:6">
       <c r="B29" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="C29" t="s">
         <v>38</v>
       </c>
       <c r="D29" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E29" t="s">
         <v>46</v>
       </c>
       <c r="F29" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="2:6">
       <c r="B30" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="C30" t="s">
         <v>38</v>
       </c>
       <c r="D30" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E30" t="s">
         <v>46</v>
       </c>
       <c r="F30" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="2:6">
       <c r="B31" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="C31" t="s">
         <v>38</v>
       </c>
       <c r="D31" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E31" t="s">
         <v>46</v>
       </c>
       <c r="F31" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="2:6">
       <c r="B32" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="C32" t="s">
         <v>38</v>
       </c>
       <c r="D32" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E32" t="s">
         <v>46</v>
       </c>
       <c r="F32" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="2:6">
       <c r="B33" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="C33" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D33" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E33" t="s">
         <v>46</v>
       </c>
       <c r="F33" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="C34" t="s">
         <v>38</v>
@@ -2373,12 +2376,12 @@
         <v>46</v>
       </c>
       <c r="F34" t="s">
-        <v>90</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="C35" t="s">
         <v>38</v>
@@ -2390,12 +2393,12 @@
         <v>46</v>
       </c>
       <c r="F35" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
       <c r="C36" t="s">
         <v>38</v>
@@ -2407,12 +2410,12 @@
         <v>46</v>
       </c>
       <c r="F36" t="s">
-        <v>90</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="C37" t="s">
         <v>38</v>
@@ -2424,46 +2427,46 @@
         <v>46</v>
       </c>
       <c r="F37" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="C38" t="s">
         <v>38</v>
       </c>
       <c r="D38" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E38" t="s">
         <v>46</v>
       </c>
       <c r="F38" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>94</v>
+        <v>127</v>
       </c>
       <c r="C39" t="s">
         <v>38</v>
       </c>
       <c r="D39" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E39" t="s">
         <v>46</v>
       </c>
       <c r="F39" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>95</v>
+        <v>128</v>
       </c>
       <c r="C40" t="s">
         <v>38</v>
@@ -2475,12 +2478,12 @@
         <v>46</v>
       </c>
       <c r="F40" t="s">
-        <v>90</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>96</v>
+        <v>130</v>
       </c>
       <c r="C41" t="s">
         <v>38</v>
@@ -2492,35 +2495,35 @@
         <v>46</v>
       </c>
       <c r="F41" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="s">
-        <v>97</v>
+        <v>131</v>
       </c>
       <c r="C42" t="s">
         <v>38</v>
       </c>
       <c r="D42" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E42" t="s">
         <v>46</v>
       </c>
       <c r="F42" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>98</v>
+        <v>141</v>
       </c>
       <c r="C43" t="s">
         <v>38</v>
       </c>
       <c r="D43" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E43" t="s">
         <v>46</v>
@@ -2529,618 +2532,42 @@
         <v>49</v>
       </c>
     </row>
-    <row r="44">
-      <c r="B44" t="s">
-        <v>99</v>
-      </c>
-      <c r="C44" t="s">
-        <v>38</v>
-      </c>
-      <c r="D44" t="s">
-        <v>48</v>
-      </c>
-      <c r="E44" t="s">
-        <v>46</v>
-      </c>
-      <c r="F44" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="B45" t="s">
-        <v>100</v>
-      </c>
-      <c r="C45" t="s">
-        <v>38</v>
-      </c>
-      <c r="D45" t="s">
-        <v>48</v>
-      </c>
-      <c r="E45" t="s">
-        <v>46</v>
-      </c>
-      <c r="F45" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="B46" t="s">
-        <v>101</v>
-      </c>
-      <c r="C46" t="s">
-        <v>38</v>
-      </c>
-      <c r="D46" t="s">
-        <v>48</v>
-      </c>
-      <c r="E46" t="s">
-        <v>46</v>
-      </c>
-      <c r="F46" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="B47" t="s">
-        <v>102</v>
-      </c>
-      <c r="C47" t="s">
-        <v>38</v>
-      </c>
-      <c r="D47" t="s">
-        <v>48</v>
-      </c>
-      <c r="E47" t="s">
-        <v>46</v>
-      </c>
-      <c r="F47" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="B48" t="s">
-        <v>103</v>
-      </c>
-      <c r="C48" t="s">
-        <v>38</v>
-      </c>
-      <c r="D48" t="s">
-        <v>48</v>
-      </c>
-      <c r="E48" t="s">
-        <v>46</v>
-      </c>
-      <c r="F48" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="B49" t="s">
-        <v>104</v>
-      </c>
-      <c r="C49" t="s">
-        <v>38</v>
-      </c>
-      <c r="D49" t="s">
-        <v>48</v>
-      </c>
-      <c r="E49" t="s">
-        <v>46</v>
-      </c>
-      <c r="F49" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="B50" t="s">
-        <v>105</v>
-      </c>
-      <c r="C50" t="s">
-        <v>38</v>
-      </c>
-      <c r="D50" t="s">
-        <v>48</v>
-      </c>
-      <c r="E50" t="s">
-        <v>46</v>
-      </c>
-      <c r="F50" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="B51" t="s">
-        <v>106</v>
-      </c>
-      <c r="C51" t="s">
-        <v>43</v>
-      </c>
-      <c r="D51" t="s">
-        <v>48</v>
-      </c>
-      <c r="E51" t="s">
-        <v>46</v>
-      </c>
-      <c r="F51" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="B52" t="s">
-        <v>107</v>
-      </c>
-      <c r="C52" t="s">
-        <v>38</v>
-      </c>
-      <c r="D52" t="s">
-        <v>48</v>
-      </c>
-      <c r="E52" t="s">
-        <v>46</v>
-      </c>
-      <c r="F52" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="B53" t="s">
-        <v>112</v>
-      </c>
-      <c r="C53" t="s">
-        <v>38</v>
-      </c>
-      <c r="D53" t="s">
-        <v>48</v>
-      </c>
-      <c r="E53" t="s">
-        <v>46</v>
-      </c>
-      <c r="F53" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="B54" t="s">
-        <v>114</v>
-      </c>
-      <c r="C54" t="s">
-        <v>38</v>
-      </c>
-      <c r="D54" t="s">
-        <v>48</v>
-      </c>
-      <c r="E54" t="s">
-        <v>46</v>
-      </c>
-      <c r="F54" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="B55" t="s">
-        <v>116</v>
-      </c>
-      <c r="C55" t="s">
-        <v>38</v>
-      </c>
-      <c r="D55" t="s">
-        <v>48</v>
-      </c>
-      <c r="E55" t="s">
-        <v>46</v>
-      </c>
-      <c r="F55" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="B56" t="s">
-        <v>117</v>
-      </c>
-      <c r="C56" t="s">
-        <v>38</v>
-      </c>
-      <c r="D56" t="s">
-        <v>45</v>
-      </c>
-      <c r="E56" t="s">
-        <v>46</v>
-      </c>
-      <c r="F56" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="B57" t="s">
-        <v>118</v>
-      </c>
-      <c r="C57" t="s">
-        <v>38</v>
-      </c>
-      <c r="D57" t="s">
-        <v>45</v>
-      </c>
-      <c r="E57" t="s">
-        <v>46</v>
-      </c>
-      <c r="F57" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="B58" t="s">
-        <v>119</v>
-      </c>
-      <c r="C58" t="s">
-        <v>38</v>
-      </c>
-      <c r="D58" t="s">
-        <v>45</v>
-      </c>
-      <c r="E58" t="s">
-        <v>46</v>
-      </c>
-      <c r="F58" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="B59" t="s">
-        <v>120</v>
-      </c>
-      <c r="C59" t="s">
-        <v>38</v>
-      </c>
-      <c r="D59" t="s">
-        <v>45</v>
-      </c>
-      <c r="E59" t="s">
-        <v>46</v>
-      </c>
-      <c r="F59" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="B60" t="s">
-        <v>121</v>
-      </c>
-      <c r="C60" t="s">
-        <v>38</v>
-      </c>
-      <c r="D60" t="s">
-        <v>45</v>
-      </c>
-      <c r="E60" t="s">
-        <v>46</v>
-      </c>
-      <c r="F60" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="B61" t="s">
-        <v>122</v>
-      </c>
-      <c r="C61" t="s">
-        <v>38</v>
-      </c>
-      <c r="D61" t="s">
-        <v>45</v>
-      </c>
-      <c r="E61" t="s">
-        <v>46</v>
-      </c>
-      <c r="F61" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="B62" t="s">
-        <v>123</v>
-      </c>
-      <c r="C62" t="s">
-        <v>38</v>
-      </c>
-      <c r="D62" t="s">
-        <v>45</v>
-      </c>
-      <c r="E62" t="s">
-        <v>46</v>
-      </c>
-      <c r="F62" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="B63" t="s">
-        <v>124</v>
-      </c>
-      <c r="C63" t="s">
-        <v>38</v>
-      </c>
-      <c r="D63" t="s">
-        <v>45</v>
-      </c>
-      <c r="E63" t="s">
-        <v>46</v>
-      </c>
-      <c r="F63" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="B64" t="s">
-        <v>125</v>
-      </c>
-      <c r="C64" t="s">
-        <v>38</v>
-      </c>
-      <c r="D64" t="s">
-        <v>45</v>
-      </c>
-      <c r="E64" t="s">
-        <v>46</v>
-      </c>
-      <c r="F64" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="B65" t="s">
-        <v>126</v>
-      </c>
-      <c r="C65" t="s">
-        <v>38</v>
-      </c>
-      <c r="D65" t="s">
-        <v>45</v>
-      </c>
-      <c r="E65" t="s">
-        <v>46</v>
-      </c>
-      <c r="F65" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="B66" t="s">
-        <v>127</v>
-      </c>
-      <c r="C66" t="s">
-        <v>38</v>
-      </c>
-      <c r="D66" t="s">
-        <v>45</v>
-      </c>
-      <c r="E66" t="s">
-        <v>46</v>
-      </c>
-      <c r="F66" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="B67" t="s">
-        <v>128</v>
-      </c>
-      <c r="C67" t="s">
-        <v>38</v>
-      </c>
-      <c r="D67" t="s">
-        <v>48</v>
-      </c>
-      <c r="E67" t="s">
-        <v>46</v>
-      </c>
-      <c r="F67" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="B68" t="s">
-        <v>130</v>
-      </c>
-      <c r="C68" t="s">
-        <v>38</v>
-      </c>
-      <c r="D68" t="s">
-        <v>48</v>
-      </c>
-      <c r="E68" t="s">
-        <v>46</v>
-      </c>
-      <c r="F68" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="B69" t="s">
-        <v>131</v>
-      </c>
-      <c r="C69" t="s">
-        <v>38</v>
-      </c>
-      <c r="D69" t="s">
-        <v>45</v>
-      </c>
-      <c r="E69" t="s">
-        <v>46</v>
-      </c>
-      <c r="F69" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="B70" t="s">
-        <v>132</v>
-      </c>
-      <c r="C70" t="s">
-        <v>38</v>
-      </c>
-      <c r="D70" t="s">
-        <v>45</v>
-      </c>
-      <c r="E70" t="s">
-        <v>46</v>
-      </c>
-      <c r="F70" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="B71" t="s">
-        <v>133</v>
-      </c>
-      <c r="C71" t="s">
-        <v>38</v>
-      </c>
-      <c r="D71" t="s">
-        <v>45</v>
-      </c>
-      <c r="E71" t="s">
-        <v>46</v>
-      </c>
-      <c r="F71" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="B72" t="s">
-        <v>134</v>
-      </c>
-      <c r="C72" t="s">
-        <v>38</v>
-      </c>
-      <c r="D72" t="s">
-        <v>45</v>
-      </c>
-      <c r="E72" t="s">
-        <v>46</v>
-      </c>
-      <c r="F72" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="B73" t="s">
-        <v>135</v>
-      </c>
-      <c r="C73" t="s">
-        <v>38</v>
-      </c>
-      <c r="D73" t="s">
-        <v>45</v>
-      </c>
-      <c r="E73" t="s">
-        <v>46</v>
-      </c>
-      <c r="F73" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="B74" t="s">
-        <v>136</v>
-      </c>
-      <c r="C74" t="s">
-        <v>38</v>
-      </c>
-      <c r="D74" t="s">
-        <v>45</v>
-      </c>
-      <c r="E74" t="s">
-        <v>46</v>
-      </c>
-      <c r="F74" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="B75" t="s">
-        <v>137</v>
-      </c>
-      <c r="C75" t="s">
-        <v>38</v>
-      </c>
-      <c r="D75" t="s">
-        <v>45</v>
-      </c>
-      <c r="E75" t="s">
-        <v>46</v>
-      </c>
-      <c r="F75" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="B76" t="s">
-        <v>138</v>
-      </c>
-      <c r="C76" t="s">
-        <v>38</v>
-      </c>
-      <c r="D76" t="s">
-        <v>45</v>
-      </c>
-      <c r="E76" t="s">
-        <v>46</v>
-      </c>
-      <c r="F76" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="B77" t="s">
-        <v>139</v>
-      </c>
-      <c r="C77" t="s">
-        <v>38</v>
-      </c>
-      <c r="D77" t="s">
-        <v>45</v>
-      </c>
-      <c r="E77" t="s">
-        <v>46</v>
-      </c>
-      <c r="F77" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="B78" t="s">
-        <v>140</v>
-      </c>
-      <c r="C78" t="s">
-        <v>38</v>
-      </c>
-      <c r="D78" t="s">
-        <v>45</v>
-      </c>
-      <c r="E78" t="s">
-        <v>46</v>
-      </c>
-      <c r="F78" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="B79" t="s">
-        <v>141</v>
-      </c>
-      <c r="C79" t="s">
-        <v>38</v>
-      </c>
-      <c r="D79" t="s">
-        <v>45</v>
-      </c>
-      <c r="E79" t="s">
-        <v>46</v>
-      </c>
-      <c r="F79" t="s">
-        <v>49</v>
-      </c>
-    </row>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56"/>
+    <row r="57"/>
+    <row r="58"/>
+    <row r="59"/>
+    <row r="60"/>
+    <row r="61"/>
+    <row r="62"/>
+    <row r="63"/>
+    <row r="64"/>
+    <row r="65"/>
+    <row r="66"/>
+    <row r="67"/>
+    <row r="68"/>
+    <row r="69"/>
+    <row r="70"/>
+    <row r="71"/>
+    <row r="72"/>
+    <row r="73"/>
+    <row r="74"/>
+    <row r="75"/>
+    <row r="76"/>
+    <row r="77"/>
+    <row r="78"/>
+    <row r="79"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>